<commit_message>
started to integrate Guille review
</commit_message>
<xml_diff>
--- a/figures/NonOptTierGraph.xlsx
+++ b/figures/NonOptTierGraph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17000" yWindow="3480" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="5600" yWindow="3760" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -289,11 +289,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2122416808"/>
-        <c:axId val="-2123096408"/>
+        <c:axId val="2090584904"/>
+        <c:axId val="2091711064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122416808"/>
+        <c:axId val="2090584904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -302,7 +302,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123096408"/>
+        <c:crossAx val="2091711064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -310,7 +310,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123096408"/>
+        <c:axId val="2091711064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -321,7 +321,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122416808"/>
+        <c:crossAx val="2090584904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -385,7 +385,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="plus"/>
+            <c:symbol val="star"/>
             <c:size val="8"/>
             <c:spPr>
               <a:ln w="12700" cmpd="sng">
@@ -519,11 +519,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2113284616"/>
-        <c:axId val="-2109757432"/>
+        <c:axId val="2090592456"/>
+        <c:axId val="2090599992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2113284616"/>
+        <c:axId val="2090592456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,7 +556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109757432"/>
+        <c:crossAx val="2090599992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -564,7 +564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109757432"/>
+        <c:axId val="2090599992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,7 +599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113284616"/>
+        <c:crossAx val="2090592456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1021,7 +1021,7 @@
   <dimension ref="B5:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>